<commit_message>
Added Evaluation testData file
</commit_message>
<xml_diff>
--- a/testdata/Certification.xlsx
+++ b/testdata/Certification.xlsx
@@ -5,21 +5,23 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chetan-cwali\eclipse-workspace\TVR_E2E_AUTOMATION\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chetan-cwali\OneDrive - Nagarro\Desktop\New folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{7322509E-4DDF-4685-825A-717411A2B564}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{A6D26505-39CB-4A11-9E70-DA0513C031ED}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView activeTab="1" windowHeight="10300" windowWidth="19420" xWindow="-110" xr2:uid="{4D26E08E-7238-3B4F-810D-4CEF30C0601E}" yWindow="-110"/>
+    <workbookView activeTab="2" windowHeight="10300" windowWidth="19420" xWindow="-110" xr2:uid="{4D26E08E-7238-3B4F-810D-4CEF30C0601E}" yWindow="-110"/>
   </bookViews>
   <sheets>
-    <sheet name="vehical" r:id="rId1" sheetId="2"/>
-    <sheet name="Engine" r:id="rId2" sheetId="28"/>
+    <sheet name="Pending_Certi_List" r:id="rId1" sheetId="34"/>
+    <sheet name="Start_Certification" r:id="rId2" sheetId="35"/>
     <sheet name="genericImage" r:id="rId3" sheetId="33"/>
-    <sheet name="Functions" r:id="rId4" sheetId="29"/>
-    <sheet name="Frames" r:id="rId5" sheetId="30"/>
-    <sheet name="Refurbishment_Cost" r:id="rId6" sheetId="32"/>
-    <sheet name="Rating_And_Pricing" r:id="rId7" sheetId="31"/>
+    <sheet name="vehical" r:id="rId4" sheetId="2"/>
+    <sheet name="Engine" r:id="rId5" sheetId="28"/>
+    <sheet name="Functions" r:id="rId6" sheetId="29"/>
+    <sheet name="Frames" r:id="rId7" sheetId="30"/>
+    <sheet name="Refurbishment_Cost" r:id="rId8" sheetId="32"/>
+    <sheet name="Rating_And_Pricing" r:id="rId9" sheetId="31"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="410">
   <si>
     <t>endpoint</t>
   </si>
@@ -729,6 +731,549 @@
   </si>
   <si>
     <t>financial_name_other</t>
+  </si>
+  <si>
+    <t>parent_grp</t>
+  </si>
+  <si>
+    <t>dealer_map_cd</t>
+  </si>
+  <si>
+    <t>loc_cd</t>
+  </si>
+  <si>
+    <t>comp_fa</t>
+  </si>
+  <si>
+    <t>fromDate</t>
+  </si>
+  <si>
+    <t>toDate</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>trvVehicle</t>
+  </si>
+  <si>
+    <t>msilVehicle</t>
+  </si>
+  <si>
+    <t>vehicleRegistrationNumber</t>
+  </si>
+  <si>
+    <t>vinNo</t>
+  </si>
+  <si>
+    <t>chasisNo</t>
+  </si>
+  <si>
+    <t>engineNo</t>
+  </si>
+  <si>
+    <t>modelDesc</t>
+  </si>
+  <si>
+    <t>variant</t>
+  </si>
+  <si>
+    <t>manufacturerCode</t>
+  </si>
+  <si>
+    <t>model</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>ewValidUpto</t>
+  </si>
+  <si>
+    <t>tvWarValidUpto</t>
+  </si>
+  <si>
+    <t>scrapFlag</t>
+  </si>
+  <si>
+    <t>certStatus</t>
+  </si>
+  <si>
+    <t>buyingId</t>
+  </si>
+  <si>
+    <t>rfSubmissionDate</t>
+  </si>
+  <si>
+    <t>evaluatorName</t>
+  </si>
+  <si>
+    <t>evaluatedRFCost</t>
+  </si>
+  <si>
+    <t>actualRFCost</t>
+  </si>
+  <si>
+    <t>referencePRice</t>
+  </si>
+  <si>
+    <t>sellPrice</t>
+  </si>
+  <si>
+    <t>dealerCode</t>
+  </si>
+  <si>
+    <t>dealerMulCode</t>
+  </si>
+  <si>
+    <t>dealerMappedCode</t>
+  </si>
+  <si>
+    <t>rejectionReason</t>
+  </si>
+  <si>
+    <t>certificationDate</t>
+  </si>
+  <si>
+    <t>buyingDate</t>
+  </si>
+  <si>
+    <t>comments</t>
+  </si>
+  <si>
+    <t>pending-certifications-list</t>
+  </si>
+  <si>
+    <t>Pending certification details fetched successfully.</t>
+  </si>
+  <si>
+    <t>ROHAN</t>
+  </si>
+  <si>
+    <t>50353</t>
+  </si>
+  <si>
+    <t>MKN</t>
+  </si>
+  <si>
+    <t>ROHA</t>
+  </si>
+  <si>
+    <t>2023-09-01</t>
+  </si>
+  <si>
+    <t>2023-11-05</t>
+  </si>
+  <si>
+    <t>RF</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>MA3EZDE1S00194969</t>
+  </si>
+  <si>
+    <t>194969</t>
+  </si>
+  <si>
+    <t>1877558</t>
+  </si>
+  <si>
+    <t>ALTO K10</t>
+  </si>
+  <si>
+    <t>ALTO K10 VXI</t>
+  </si>
+  <si>
+    <t>MARUTI</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>AK</t>
+  </si>
+  <si>
+    <t>AKR4CD3</t>
+  </si>
+  <si>
+    <t>SILKY SILVER</t>
+  </si>
+  <si>
+    <t>Z2S</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>1168099</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>B23013042779</t>
+  </si>
+  <si>
+    <t>ROHIT KUMAR YADAV</t>
+  </si>
+  <si>
+    <t>170000.0</t>
+  </si>
+  <si>
+    <t>225000</t>
+  </si>
+  <si>
+    <t>59NA</t>
+  </si>
+  <si>
+    <t>07 Sep 2023, 15:42</t>
+  </si>
+  <si>
+    <t>06 Sep 2023, 12:38</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>HR10AD7035</t>
+  </si>
+  <si>
+    <t>MA3NYFB1SHK293624</t>
+  </si>
+  <si>
+    <t>293624</t>
+  </si>
+  <si>
+    <t>5523245</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VITARA BREZZA </t>
+  </si>
+  <si>
+    <t>MARUTI VITARA BREZZA VDI (O)</t>
+  </si>
+  <si>
+    <t>VB</t>
+  </si>
+  <si>
+    <t>VBRDAVA</t>
+  </si>
+  <si>
+    <t>PEARL  ARCTIC WHITE</t>
+  </si>
+  <si>
+    <t>ZHJ</t>
+  </si>
+  <si>
+    <t>B23012889356</t>
+  </si>
+  <si>
+    <t>510000.0</t>
+  </si>
+  <si>
+    <t>565000</t>
+  </si>
+  <si>
+    <t>22 Sep 2023, 10:21</t>
+  </si>
+  <si>
+    <t>09 Aug 2023, 10:55</t>
+  </si>
+  <si>
+    <t>DL2CAU5169</t>
+  </si>
+  <si>
+    <t>MA3EXMG1S00115619</t>
+  </si>
+  <si>
+    <t>115619</t>
+  </si>
+  <si>
+    <t>7055705</t>
+  </si>
+  <si>
+    <t>CIAZ</t>
+  </si>
+  <si>
+    <t>MARUTI CIAZ VXI</t>
+  </si>
+  <si>
+    <t>CI</t>
+  </si>
+  <si>
+    <t>CIR4CD1</t>
+  </si>
+  <si>
+    <t>PRL.SANGRIA RED</t>
+  </si>
+  <si>
+    <t>ZQL</t>
+  </si>
+  <si>
+    <t>1069530</t>
+  </si>
+  <si>
+    <t>B23013229525</t>
+  </si>
+  <si>
+    <t>NARENDER KUMAR</t>
+  </si>
+  <si>
+    <t>325000.0</t>
+  </si>
+  <si>
+    <t>0-0</t>
+  </si>
+  <si>
+    <t>395000</t>
+  </si>
+  <si>
+    <t>5904</t>
+  </si>
+  <si>
+    <t>09 Oct 2023, 11:44</t>
+  </si>
+  <si>
+    <t>08 Oct 2023, 16:34</t>
+  </si>
+  <si>
+    <t>UP14BZ8788</t>
+  </si>
+  <si>
+    <t>MA3FHEB1S00465221</t>
+  </si>
+  <si>
+    <t>465221</t>
+  </si>
+  <si>
+    <t>401475</t>
+  </si>
+  <si>
+    <t>NEW SWIFT</t>
+  </si>
+  <si>
+    <t>MARUTI SWIFT VDI</t>
+  </si>
+  <si>
+    <t>SM</t>
+  </si>
+  <si>
+    <t>SMRDCD1</t>
+  </si>
+  <si>
+    <t>715209</t>
+  </si>
+  <si>
+    <t>B23013237734</t>
+  </si>
+  <si>
+    <t>GAGAN SAXENA</t>
+  </si>
+  <si>
+    <t>120000.0</t>
+  </si>
+  <si>
+    <t>210463-272822</t>
+  </si>
+  <si>
+    <t>185000</t>
+  </si>
+  <si>
+    <t>09 Oct 2023, 11:53</t>
+  </si>
+  <si>
+    <t>08 Oct 2023, 17:13</t>
+  </si>
+  <si>
+    <t>UP14DW3873</t>
+  </si>
+  <si>
+    <t>MA3EUA61S00D44927</t>
+  </si>
+  <si>
+    <t>D44927</t>
+  </si>
+  <si>
+    <t>6101990</t>
+  </si>
+  <si>
+    <t>ALTO 800</t>
+  </si>
+  <si>
+    <t>MARUTI ALTO 800 GREEN LXI</t>
+  </si>
+  <si>
+    <t>AN</t>
+  </si>
+  <si>
+    <t>ANRCCS7</t>
+  </si>
+  <si>
+    <t>SUPERIOR WHITE</t>
+  </si>
+  <si>
+    <t>26U</t>
+  </si>
+  <si>
+    <t>B23013049214</t>
+  </si>
+  <si>
+    <t>220000.0</t>
+  </si>
+  <si>
+    <t>285000</t>
+  </si>
+  <si>
+    <t>15 Oct 2023, 11:55</t>
+  </si>
+  <si>
+    <t>08 Oct 2023, 16:42</t>
+  </si>
+  <si>
+    <t>UP14CK9184</t>
+  </si>
+  <si>
+    <t>MA3EUA61S00422197</t>
+  </si>
+  <si>
+    <t>422197</t>
+  </si>
+  <si>
+    <t>5206335</t>
+  </si>
+  <si>
+    <t>MARUTI ALTO 800 LXI BS IV</t>
+  </si>
+  <si>
+    <t>ANR4CS3</t>
+  </si>
+  <si>
+    <t>B23013385692</t>
+  </si>
+  <si>
+    <t>112510-145847</t>
+  </si>
+  <si>
+    <t>195000</t>
+  </si>
+  <si>
+    <t>29 Oct 2023, 10:49</t>
+  </si>
+  <si>
+    <t>29 Oct 2023, 10:13</t>
+  </si>
+  <si>
+    <t>DL9CX2345</t>
+  </si>
+  <si>
+    <t>MA3EKE42S00177599</t>
+  </si>
+  <si>
+    <t>177599</t>
+  </si>
+  <si>
+    <t>497226</t>
+  </si>
+  <si>
+    <t>SWIFT DZIRE</t>
+  </si>
+  <si>
+    <t>MARUTI SWIFT DZIRE VXI (BHARAT STAGE III)</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>SR4CD1</t>
+  </si>
+  <si>
+    <t>BRIGHT RED</t>
+  </si>
+  <si>
+    <t>Z9T</t>
+  </si>
+  <si>
+    <t>B23012808040</t>
+  </si>
+  <si>
+    <t>75000.0</t>
+  </si>
+  <si>
+    <t>105000</t>
+  </si>
+  <si>
+    <t>6G01</t>
+  </si>
+  <si>
+    <t>03 Nov 2023, 10:12</t>
+  </si>
+  <si>
+    <t>09 Aug 2023, 14:32</t>
+  </si>
+  <si>
+    <t>parentGroup</t>
+  </si>
+  <si>
+    <t>certificationNumber</t>
+  </si>
+  <si>
+    <t>manufacturerName</t>
+  </si>
+  <si>
+    <t>chassisNo</t>
+  </si>
+  <si>
+    <t>regNo</t>
+  </si>
+  <si>
+    <t>modelName</t>
+  </si>
+  <si>
+    <t>variantName</t>
+  </si>
+  <si>
+    <t>rfDate</t>
+  </si>
+  <si>
+    <t>start/certification</t>
+  </si>
+  <si>
+    <t>This record is already submitted by 1051756</t>
+  </si>
+  <si>
+    <t>59TB-59:MKN</t>
+  </si>
+  <si>
+    <t>re</t>
+  </si>
+  <si>
+    <t>CERT-25092023-000079MPN1168099</t>
+  </si>
+  <si>
+    <t>04 Sep 2023, 10:09</t>
+  </si>
+  <si>
+    <t>CERT-01112023-000100MPN1069530</t>
+  </si>
+  <si>
+    <t>MSPIN is mandatory</t>
+  </si>
+  <si>
+    <t>CERT-22112023-000122MPN715209</t>
+  </si>
+  <si>
+    <t>Something went wrong</t>
+  </si>
+  <si>
+    <t>Certification submission in progress. Please wait.</t>
   </si>
 </sst>
 </file>
@@ -736,7 +1281,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -755,6 +1300,13 @@
       <color rgb="FF000000"/>
       <name val="Menlo"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9CDCFE"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -806,7 +1358,7 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="27">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
@@ -853,6 +1405,15 @@
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" quotePrefix="1" xfId="0"/>
     <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" quotePrefix="1" xfId="0"/>
     <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" quotePrefix="1" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -1167,6 +1728,1766 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56886EAE-986F-4CD2-ABDD-A328FB0E7115}">
+  <dimension ref="A1:AX8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:AW8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.5"/>
+  <sheetData>
+    <row r="1" spans="1:49">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>229</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>230</v>
+      </c>
+      <c r="F1" t="s">
+        <v>231</v>
+      </c>
+      <c r="G1" t="s">
+        <v>232</v>
+      </c>
+      <c r="H1" s="24" t="s">
+        <v>233</v>
+      </c>
+      <c r="I1" t="s">
+        <v>234</v>
+      </c>
+      <c r="J1" t="s">
+        <v>235</v>
+      </c>
+      <c r="K1" t="s">
+        <v>236</v>
+      </c>
+      <c r="L1" t="s">
+        <v>237</v>
+      </c>
+      <c r="M1" t="s">
+        <v>238</v>
+      </c>
+      <c r="N1" t="s">
+        <v>239</v>
+      </c>
+      <c r="O1" t="s">
+        <v>240</v>
+      </c>
+      <c r="P1" t="s">
+        <v>241</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>242</v>
+      </c>
+      <c r="R1" t="s">
+        <v>243</v>
+      </c>
+      <c r="S1" t="s">
+        <v>174</v>
+      </c>
+      <c r="T1" t="s">
+        <v>244</v>
+      </c>
+      <c r="U1" t="s">
+        <v>245</v>
+      </c>
+      <c r="V1" t="s">
+        <v>171</v>
+      </c>
+      <c r="W1" t="s">
+        <v>172</v>
+      </c>
+      <c r="X1" t="s">
+        <v>246</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>173</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>236</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>135</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>247</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>248</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>249</v>
+      </c>
+      <c r="AE1" s="25" t="s">
+        <v>250</v>
+      </c>
+      <c r="AF1" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="AG1" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH1" s="25" t="s">
+        <v>251</v>
+      </c>
+      <c r="AI1" s="25" t="s">
+        <v>252</v>
+      </c>
+      <c r="AJ1" s="25" t="s">
+        <v>253</v>
+      </c>
+      <c r="AK1" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="AL1" s="25" t="s">
+        <v>254</v>
+      </c>
+      <c r="AM1" s="25" t="s">
+        <v>255</v>
+      </c>
+      <c r="AN1" s="25" t="s">
+        <v>256</v>
+      </c>
+      <c r="AO1" s="25" t="s">
+        <v>257</v>
+      </c>
+      <c r="AP1" s="25" t="s">
+        <v>258</v>
+      </c>
+      <c r="AQ1" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="AR1" s="25" t="s">
+        <v>259</v>
+      </c>
+      <c r="AS1" s="25" t="s">
+        <v>260</v>
+      </c>
+      <c r="AT1" s="25" t="s">
+        <v>261</v>
+      </c>
+      <c r="AU1" s="25" t="s">
+        <v>262</v>
+      </c>
+      <c r="AV1" s="25" t="s">
+        <v>263</v>
+      </c>
+      <c r="AW1" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="2" spans="1:49">
+      <c r="A2" t="s">
+        <v>265</v>
+      </c>
+      <c r="B2" t="s">
+        <v>266</v>
+      </c>
+      <c r="D2" t="s">
+        <v>267</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>268</v>
+      </c>
+      <c r="F2" t="s">
+        <v>269</v>
+      </c>
+      <c r="G2" t="s">
+        <v>270</v>
+      </c>
+      <c r="H2" s="26" t="s">
+        <v>271</v>
+      </c>
+      <c r="I2" s="26" t="s">
+        <v>272</v>
+      </c>
+      <c r="J2" t="s">
+        <v>273</v>
+      </c>
+      <c r="K2" t="s">
+        <v>274</v>
+      </c>
+      <c r="L2" t="b">
+        <v>1</v>
+      </c>
+      <c r="M2" t="s">
+        <v>159</v>
+      </c>
+      <c r="N2" t="s">
+        <v>275</v>
+      </c>
+      <c r="O2" t="s">
+        <v>276</v>
+      </c>
+      <c r="P2" t="s">
+        <v>277</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>278</v>
+      </c>
+      <c r="R2" t="s">
+        <v>279</v>
+      </c>
+      <c r="S2" t="s">
+        <v>280</v>
+      </c>
+      <c r="T2" t="s">
+        <v>281</v>
+      </c>
+      <c r="U2" t="s">
+        <v>278</v>
+      </c>
+      <c r="V2" t="s">
+        <v>282</v>
+      </c>
+      <c r="W2" t="s">
+        <v>283</v>
+      </c>
+      <c r="X2" t="s">
+        <v>284</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>285</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>286</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>287</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>287</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>287</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>288</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>289</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>290</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>291</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>292</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>293</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>290</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>129</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>287</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>294</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>295</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>268</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>296</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>297</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="3" spans="1:49">
+      <c r="M3" t="s">
+        <v>299</v>
+      </c>
+      <c r="N3" t="s">
+        <v>300</v>
+      </c>
+      <c r="O3" t="s">
+        <v>301</v>
+      </c>
+      <c r="P3" t="s">
+        <v>302</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>303</v>
+      </c>
+      <c r="R3" t="s">
+        <v>304</v>
+      </c>
+      <c r="S3" t="s">
+        <v>280</v>
+      </c>
+      <c r="T3" t="s">
+        <v>281</v>
+      </c>
+      <c r="U3" t="s">
+        <v>303</v>
+      </c>
+      <c r="V3" t="s">
+        <v>305</v>
+      </c>
+      <c r="W3" t="s">
+        <v>306</v>
+      </c>
+      <c r="X3" t="s">
+        <v>307</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>308</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>286</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>287</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>287</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>287</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>288</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>289</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>290</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>309</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>292</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>310</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>290</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>129</v>
+      </c>
+      <c r="AN3" t="s">
+        <v>287</v>
+      </c>
+      <c r="AO3" t="s">
+        <v>311</v>
+      </c>
+      <c r="AR3" t="s">
+        <v>295</v>
+      </c>
+      <c r="AS3" t="s">
+        <v>268</v>
+      </c>
+      <c r="AU3" t="s">
+        <v>312</v>
+      </c>
+      <c r="AV3" t="s">
+        <v>313</v>
+      </c>
+      <c r="AW3" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="4" spans="1:49">
+      <c r="M4" t="s">
+        <v>314</v>
+      </c>
+      <c r="N4" t="s">
+        <v>315</v>
+      </c>
+      <c r="O4" t="s">
+        <v>316</v>
+      </c>
+      <c r="P4" t="s">
+        <v>317</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>318</v>
+      </c>
+      <c r="R4" t="s">
+        <v>319</v>
+      </c>
+      <c r="S4" t="s">
+        <v>280</v>
+      </c>
+      <c r="T4" t="s">
+        <v>281</v>
+      </c>
+      <c r="U4" t="s">
+        <v>318</v>
+      </c>
+      <c r="V4" t="s">
+        <v>320</v>
+      </c>
+      <c r="W4" t="s">
+        <v>321</v>
+      </c>
+      <c r="X4" t="s">
+        <v>322</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>323</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>286</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>287</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>287</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>287</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>288</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>324</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>290</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>325</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>326</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>327</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>290</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>162</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>328</v>
+      </c>
+      <c r="AO4" t="s">
+        <v>329</v>
+      </c>
+      <c r="AR4" t="s">
+        <v>330</v>
+      </c>
+      <c r="AS4" t="s">
+        <v>268</v>
+      </c>
+      <c r="AU4" t="s">
+        <v>331</v>
+      </c>
+      <c r="AV4" t="s">
+        <v>332</v>
+      </c>
+      <c r="AW4" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="5" spans="1:49">
+      <c r="M5" t="s">
+        <v>333</v>
+      </c>
+      <c r="N5" t="s">
+        <v>334</v>
+      </c>
+      <c r="O5" t="s">
+        <v>335</v>
+      </c>
+      <c r="P5" t="s">
+        <v>336</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>337</v>
+      </c>
+      <c r="R5" t="s">
+        <v>338</v>
+      </c>
+      <c r="S5" t="s">
+        <v>280</v>
+      </c>
+      <c r="T5" t="s">
+        <v>281</v>
+      </c>
+      <c r="U5" t="s">
+        <v>337</v>
+      </c>
+      <c r="V5" t="s">
+        <v>339</v>
+      </c>
+      <c r="W5" t="s">
+        <v>340</v>
+      </c>
+      <c r="X5" t="s">
+        <v>307</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>308</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>286</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>287</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>287</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>287</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>288</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>341</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>290</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>342</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>343</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>344</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>290</v>
+      </c>
+      <c r="AM5" t="s">
+        <v>163</v>
+      </c>
+      <c r="AN5" t="s">
+        <v>345</v>
+      </c>
+      <c r="AO5" t="s">
+        <v>346</v>
+      </c>
+      <c r="AR5" t="s">
+        <v>330</v>
+      </c>
+      <c r="AS5" t="s">
+        <v>268</v>
+      </c>
+      <c r="AU5" t="s">
+        <v>347</v>
+      </c>
+      <c r="AV5" t="s">
+        <v>348</v>
+      </c>
+      <c r="AW5" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="6" spans="1:49">
+      <c r="M6" t="s">
+        <v>349</v>
+      </c>
+      <c r="N6" t="s">
+        <v>350</v>
+      </c>
+      <c r="O6" t="s">
+        <v>351</v>
+      </c>
+      <c r="P6" t="s">
+        <v>352</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>353</v>
+      </c>
+      <c r="R6" t="s">
+        <v>354</v>
+      </c>
+      <c r="S6" t="s">
+        <v>280</v>
+      </c>
+      <c r="T6" t="s">
+        <v>281</v>
+      </c>
+      <c r="U6" t="s">
+        <v>353</v>
+      </c>
+      <c r="V6" t="s">
+        <v>355</v>
+      </c>
+      <c r="W6" t="s">
+        <v>356</v>
+      </c>
+      <c r="X6" t="s">
+        <v>357</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>358</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>286</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>287</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>287</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>287</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>288</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>341</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>290</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>359</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>343</v>
+      </c>
+      <c r="AK6" t="s">
+        <v>360</v>
+      </c>
+      <c r="AL6" t="s">
+        <v>290</v>
+      </c>
+      <c r="AM6" t="s">
+        <v>129</v>
+      </c>
+      <c r="AN6" t="s">
+        <v>287</v>
+      </c>
+      <c r="AO6" t="s">
+        <v>361</v>
+      </c>
+      <c r="AR6" t="s">
+        <v>330</v>
+      </c>
+      <c r="AS6" t="s">
+        <v>268</v>
+      </c>
+      <c r="AU6" t="s">
+        <v>362</v>
+      </c>
+      <c r="AV6" t="s">
+        <v>363</v>
+      </c>
+      <c r="AW6" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="7" spans="1:49">
+      <c r="M7" t="s">
+        <v>364</v>
+      </c>
+      <c r="N7" t="s">
+        <v>365</v>
+      </c>
+      <c r="O7" t="s">
+        <v>366</v>
+      </c>
+      <c r="P7" t="s">
+        <v>367</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>353</v>
+      </c>
+      <c r="R7" t="s">
+        <v>368</v>
+      </c>
+      <c r="S7" t="s">
+        <v>280</v>
+      </c>
+      <c r="T7" t="s">
+        <v>281</v>
+      </c>
+      <c r="U7" t="s">
+        <v>353</v>
+      </c>
+      <c r="V7" t="s">
+        <v>355</v>
+      </c>
+      <c r="W7" t="s">
+        <v>369</v>
+      </c>
+      <c r="X7" t="s">
+        <v>284</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>285</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>286</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>287</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>287</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>287</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>288</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>341</v>
+      </c>
+      <c r="AG7" t="s">
+        <v>290</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>370</v>
+      </c>
+      <c r="AJ7" t="s">
+        <v>343</v>
+      </c>
+      <c r="AK7" t="s">
+        <v>344</v>
+      </c>
+      <c r="AL7" t="s">
+        <v>290</v>
+      </c>
+      <c r="AM7" t="s">
+        <v>129</v>
+      </c>
+      <c r="AN7" t="s">
+        <v>371</v>
+      </c>
+      <c r="AO7" t="s">
+        <v>372</v>
+      </c>
+      <c r="AR7" t="s">
+        <v>330</v>
+      </c>
+      <c r="AS7" t="s">
+        <v>268</v>
+      </c>
+      <c r="AU7" t="s">
+        <v>373</v>
+      </c>
+      <c r="AV7" t="s">
+        <v>374</v>
+      </c>
+      <c r="AW7" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="8" spans="1:49">
+      <c r="M8" t="s">
+        <v>375</v>
+      </c>
+      <c r="N8" t="s">
+        <v>376</v>
+      </c>
+      <c r="O8" t="s">
+        <v>377</v>
+      </c>
+      <c r="P8" t="s">
+        <v>378</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>379</v>
+      </c>
+      <c r="R8" t="s">
+        <v>380</v>
+      </c>
+      <c r="S8" t="s">
+        <v>280</v>
+      </c>
+      <c r="T8" t="s">
+        <v>281</v>
+      </c>
+      <c r="U8" t="s">
+        <v>379</v>
+      </c>
+      <c r="V8" t="s">
+        <v>381</v>
+      </c>
+      <c r="W8" t="s">
+        <v>382</v>
+      </c>
+      <c r="X8" t="s">
+        <v>383</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>384</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>286</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>287</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>287</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>287</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>288</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>287</v>
+      </c>
+      <c r="AG8" t="s">
+        <v>290</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>385</v>
+      </c>
+      <c r="AJ8" t="s">
+        <v>287</v>
+      </c>
+      <c r="AK8" t="s">
+        <v>386</v>
+      </c>
+      <c r="AL8" t="s">
+        <v>290</v>
+      </c>
+      <c r="AM8" t="s">
+        <v>129</v>
+      </c>
+      <c r="AN8" t="s">
+        <v>287</v>
+      </c>
+      <c r="AO8" t="s">
+        <v>387</v>
+      </c>
+      <c r="AR8" t="s">
+        <v>388</v>
+      </c>
+      <c r="AS8" t="s">
+        <v>268</v>
+      </c>
+      <c r="AU8" t="s">
+        <v>389</v>
+      </c>
+      <c r="AV8" t="s">
+        <v>390</v>
+      </c>
+      <c r="AW8" t="s">
+        <v>298</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{206D828C-CE46-4F19-817B-F3AF4498D275}">
+  <dimension ref="A1:AC8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.5"/>
+  <cols>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="40.52734375" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="31.59375" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1" t="s">
+        <v>391</v>
+      </c>
+      <c r="F1" t="s">
+        <v>258</v>
+      </c>
+      <c r="G1" t="s">
+        <v>253</v>
+      </c>
+      <c r="H1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I1" t="s">
+        <v>254</v>
+      </c>
+      <c r="J1" t="s">
+        <v>255</v>
+      </c>
+      <c r="K1" t="s">
+        <v>135</v>
+      </c>
+      <c r="L1" t="s">
+        <v>392</v>
+      </c>
+      <c r="M1" t="s">
+        <v>82</v>
+      </c>
+      <c r="N1" t="s">
+        <v>91</v>
+      </c>
+      <c r="O1" t="s">
+        <v>174</v>
+      </c>
+      <c r="P1" t="s">
+        <v>393</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>394</v>
+      </c>
+      <c r="R1" t="s">
+        <v>246</v>
+      </c>
+      <c r="S1" t="s">
+        <v>241</v>
+      </c>
+      <c r="T1" t="s">
+        <v>395</v>
+      </c>
+      <c r="U1" t="s">
+        <v>396</v>
+      </c>
+      <c r="V1" t="s">
+        <v>397</v>
+      </c>
+      <c r="W1" t="s">
+        <v>239</v>
+      </c>
+      <c r="X1" t="s">
+        <v>171</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>172</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>173</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>398</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28">
+      <c r="A2" t="s">
+        <v>399</v>
+      </c>
+      <c r="B2" t="s">
+        <v>400</v>
+      </c>
+      <c r="C2" t="s">
+        <v>289</v>
+      </c>
+      <c r="D2" t="s">
+        <v>291</v>
+      </c>
+      <c r="E2" t="s">
+        <v>267</v>
+      </c>
+      <c r="F2" t="s">
+        <v>401</v>
+      </c>
+      <c r="G2" t="s">
+        <v>292</v>
+      </c>
+      <c r="H2" s="23" t="s">
+        <v>293</v>
+      </c>
+      <c r="I2" s="23" t="s">
+        <v>290</v>
+      </c>
+      <c r="J2" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="K2" s="23" t="s">
+        <v>287</v>
+      </c>
+      <c r="L2" t="s">
+        <v>402</v>
+      </c>
+      <c r="M2" t="s">
+        <v>403</v>
+      </c>
+      <c r="N2" s="23" t="s">
+        <v>329</v>
+      </c>
+      <c r="O2" t="s">
+        <v>280</v>
+      </c>
+      <c r="P2" t="s">
+        <v>280</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>276</v>
+      </c>
+      <c r="R2" t="s">
+        <v>284</v>
+      </c>
+      <c r="S2" t="s">
+        <v>277</v>
+      </c>
+      <c r="T2" t="s">
+        <v>159</v>
+      </c>
+      <c r="U2" t="s">
+        <v>278</v>
+      </c>
+      <c r="V2" t="s">
+        <v>279</v>
+      </c>
+      <c r="W2" t="s">
+        <v>275</v>
+      </c>
+      <c r="X2" t="s">
+        <v>282</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>283</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>285</v>
+      </c>
+      <c r="AA2" s="23" t="s">
+        <v>404</v>
+      </c>
+      <c r="AB2" s="23" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28">
+      <c r="A3" t="s">
+        <v>399</v>
+      </c>
+      <c r="C3" t="s">
+        <v>289</v>
+      </c>
+      <c r="D3" t="s">
+        <v>309</v>
+      </c>
+      <c r="E3" t="s">
+        <v>267</v>
+      </c>
+      <c r="F3" t="s">
+        <v>401</v>
+      </c>
+      <c r="G3" t="s">
+        <v>292</v>
+      </c>
+      <c r="H3" t="s">
+        <v>310</v>
+      </c>
+      <c r="I3" t="s">
+        <v>290</v>
+      </c>
+      <c r="J3" t="s">
+        <v>129</v>
+      </c>
+      <c r="K3" t="s">
+        <v>287</v>
+      </c>
+      <c r="M3" t="s">
+        <v>405</v>
+      </c>
+      <c r="N3" s="23" t="s">
+        <v>329</v>
+      </c>
+      <c r="O3" t="s">
+        <v>280</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>301</v>
+      </c>
+      <c r="R3" t="s">
+        <v>307</v>
+      </c>
+      <c r="S3" t="s">
+        <v>302</v>
+      </c>
+      <c r="T3" t="s">
+        <v>299</v>
+      </c>
+      <c r="U3" t="s">
+        <v>303</v>
+      </c>
+      <c r="V3" t="s">
+        <v>304</v>
+      </c>
+      <c r="W3" t="s">
+        <v>300</v>
+      </c>
+      <c r="X3" t="s">
+        <v>305</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>306</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>308</v>
+      </c>
+      <c r="AA3" s="23" t="s">
+        <v>404</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28">
+      <c r="A4" t="s">
+        <v>399</v>
+      </c>
+      <c r="B4" t="s">
+        <v>406</v>
+      </c>
+      <c r="C4" t="s">
+        <v>324</v>
+      </c>
+      <c r="D4" t="s">
+        <v>325</v>
+      </c>
+      <c r="E4" t="s">
+        <v>267</v>
+      </c>
+      <c r="F4" t="s">
+        <v>401</v>
+      </c>
+      <c r="G4" t="s">
+        <v>326</v>
+      </c>
+      <c r="H4" t="s">
+        <v>327</v>
+      </c>
+      <c r="I4" t="s">
+        <v>290</v>
+      </c>
+      <c r="J4" t="s">
+        <v>162</v>
+      </c>
+      <c r="K4" t="s">
+        <v>287</v>
+      </c>
+      <c r="M4" t="s">
+        <v>407</v>
+      </c>
+      <c r="N4" s="23" t="s">
+        <v>329</v>
+      </c>
+      <c r="O4" t="s">
+        <v>280</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>316</v>
+      </c>
+      <c r="R4" t="s">
+        <v>322</v>
+      </c>
+      <c r="S4" t="s">
+        <v>317</v>
+      </c>
+      <c r="T4" t="s">
+        <v>314</v>
+      </c>
+      <c r="U4" t="s">
+        <v>318</v>
+      </c>
+      <c r="V4" t="s">
+        <v>319</v>
+      </c>
+      <c r="W4" t="s">
+        <v>315</v>
+      </c>
+      <c r="X4" t="s">
+        <v>320</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>321</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>323</v>
+      </c>
+      <c r="AA4" s="23" t="s">
+        <v>404</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28">
+      <c r="A5" t="s">
+        <v>399</v>
+      </c>
+      <c r="B5" t="s">
+        <v>406</v>
+      </c>
+      <c r="C5" t="s">
+        <v>341</v>
+      </c>
+      <c r="D5" t="s">
+        <v>342</v>
+      </c>
+      <c r="E5" t="s">
+        <v>267</v>
+      </c>
+      <c r="F5" t="s">
+        <v>401</v>
+      </c>
+      <c r="G5" t="s">
+        <v>343</v>
+      </c>
+      <c r="H5" t="s">
+        <v>344</v>
+      </c>
+      <c r="I5" t="s">
+        <v>290</v>
+      </c>
+      <c r="J5" t="s">
+        <v>163</v>
+      </c>
+      <c r="K5" t="s">
+        <v>287</v>
+      </c>
+      <c r="M5" t="s">
+        <v>290</v>
+      </c>
+      <c r="N5" s="23" t="s">
+        <v>329</v>
+      </c>
+      <c r="O5" t="s">
+        <v>280</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>335</v>
+      </c>
+      <c r="R5" t="s">
+        <v>307</v>
+      </c>
+      <c r="S5" t="s">
+        <v>336</v>
+      </c>
+      <c r="T5" t="s">
+        <v>333</v>
+      </c>
+      <c r="U5" t="s">
+        <v>337</v>
+      </c>
+      <c r="V5" t="s">
+        <v>338</v>
+      </c>
+      <c r="W5" t="s">
+        <v>334</v>
+      </c>
+      <c r="X5" t="s">
+        <v>339</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>340</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>308</v>
+      </c>
+      <c r="AA5" s="23" t="s">
+        <v>404</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28">
+      <c r="A6" t="s">
+        <v>399</v>
+      </c>
+      <c r="C6" t="s">
+        <v>341</v>
+      </c>
+      <c r="D6" t="s">
+        <v>359</v>
+      </c>
+      <c r="E6" t="s">
+        <v>267</v>
+      </c>
+      <c r="F6" t="s">
+        <v>401</v>
+      </c>
+      <c r="G6" t="s">
+        <v>343</v>
+      </c>
+      <c r="H6" t="s">
+        <v>360</v>
+      </c>
+      <c r="I6" t="s">
+        <v>290</v>
+      </c>
+      <c r="J6" t="s">
+        <v>129</v>
+      </c>
+      <c r="K6" t="s">
+        <v>287</v>
+      </c>
+      <c r="M6" t="s">
+        <v>290</v>
+      </c>
+      <c r="N6" s="23" t="s">
+        <v>329</v>
+      </c>
+      <c r="O6" t="s">
+        <v>280</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>351</v>
+      </c>
+      <c r="R6" t="s">
+        <v>357</v>
+      </c>
+      <c r="S6" t="s">
+        <v>352</v>
+      </c>
+      <c r="T6" t="s">
+        <v>349</v>
+      </c>
+      <c r="U6" t="s">
+        <v>353</v>
+      </c>
+      <c r="V6" t="s">
+        <v>354</v>
+      </c>
+      <c r="W6" t="s">
+        <v>350</v>
+      </c>
+      <c r="X6" t="s">
+        <v>355</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>356</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>358</v>
+      </c>
+      <c r="AA6" s="23" t="s">
+        <v>404</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28">
+      <c r="A7" t="s">
+        <v>399</v>
+      </c>
+      <c r="C7" t="s">
+        <v>341</v>
+      </c>
+      <c r="D7" t="s">
+        <v>370</v>
+      </c>
+      <c r="E7" t="s">
+        <v>267</v>
+      </c>
+      <c r="F7" t="s">
+        <v>401</v>
+      </c>
+      <c r="G7" t="s">
+        <v>343</v>
+      </c>
+      <c r="H7" t="s">
+        <v>344</v>
+      </c>
+      <c r="I7" t="s">
+        <v>290</v>
+      </c>
+      <c r="J7" t="s">
+        <v>129</v>
+      </c>
+      <c r="K7" t="s">
+        <v>287</v>
+      </c>
+      <c r="M7" t="s">
+        <v>290</v>
+      </c>
+      <c r="N7" s="23" t="s">
+        <v>329</v>
+      </c>
+      <c r="O7" t="s">
+        <v>280</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>366</v>
+      </c>
+      <c r="R7" t="s">
+        <v>284</v>
+      </c>
+      <c r="S7" t="s">
+        <v>367</v>
+      </c>
+      <c r="T7" t="s">
+        <v>364</v>
+      </c>
+      <c r="U7" t="s">
+        <v>353</v>
+      </c>
+      <c r="V7" t="s">
+        <v>368</v>
+      </c>
+      <c r="W7" t="s">
+        <v>365</v>
+      </c>
+      <c r="X7" t="s">
+        <v>355</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>369</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>285</v>
+      </c>
+      <c r="AA7" s="23" t="s">
+        <v>404</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28">
+      <c r="A8" t="s">
+        <v>399</v>
+      </c>
+      <c r="C8" t="s">
+        <v>287</v>
+      </c>
+      <c r="D8" t="s">
+        <v>385</v>
+      </c>
+      <c r="E8" t="s">
+        <v>267</v>
+      </c>
+      <c r="F8" t="s">
+        <v>401</v>
+      </c>
+      <c r="G8" t="s">
+        <v>287</v>
+      </c>
+      <c r="H8" t="s">
+        <v>386</v>
+      </c>
+      <c r="I8" t="s">
+        <v>290</v>
+      </c>
+      <c r="J8" t="s">
+        <v>129</v>
+      </c>
+      <c r="K8" t="s">
+        <v>287</v>
+      </c>
+      <c r="M8" t="s">
+        <v>290</v>
+      </c>
+      <c r="N8" s="23" t="s">
+        <v>329</v>
+      </c>
+      <c r="O8" t="s">
+        <v>280</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>377</v>
+      </c>
+      <c r="R8" t="s">
+        <v>383</v>
+      </c>
+      <c r="S8" t="s">
+        <v>378</v>
+      </c>
+      <c r="T8" t="s">
+        <v>375</v>
+      </c>
+      <c r="U8" t="s">
+        <v>379</v>
+      </c>
+      <c r="V8" t="s">
+        <v>380</v>
+      </c>
+      <c r="W8" t="s">
+        <v>376</v>
+      </c>
+      <c r="X8" t="s">
+        <v>381</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>382</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>384</v>
+      </c>
+      <c r="AA8" s="23" t="s">
+        <v>404</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>390</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21D1EA00-6B85-4E2C-9FB5-EA179A3143F2}">
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.5"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="32.58203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="31.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="35.83203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="42.4140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="28.1640625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="52.9140625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>124</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDA052DD-52F2-2841-8546-5818D4D729BB}">
   <dimension ref="A1:BP101"/>
   <sheetViews>
@@ -1180,7 +3501,7 @@
     <col min="2" max="2" bestFit="true" customWidth="true" width="9.5" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="7.75" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="5.75" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.25" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="31.59375" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="17.1640625" collapsed="true"/>
     <col min="7" max="7" bestFit="true" customWidth="true" width="11.4140625" collapsed="true"/>
     <col min="8" max="8" bestFit="true" customWidth="true" width="9.33203125" collapsed="true"/>
@@ -1481,16 +3802,25 @@
       <c r="A2" s="1" t="s">
         <v>95</v>
       </c>
+      <c r="E2" t="s">
+        <v>403</v>
+      </c>
       <c r="Z2"/>
       <c r="BE2"/>
       <c r="BO2"/>
     </row>
     <row r="3" spans="1:67">
+      <c r="E3" t="s">
+        <v>405</v>
+      </c>
       <c r="Z3"/>
       <c r="BE3"/>
       <c r="BO3"/>
     </row>
     <row r="4" spans="1:67">
+      <c r="E4" t="s">
+        <v>407</v>
+      </c>
       <c r="Z4"/>
       <c r="BE4"/>
       <c r="BO4"/>
@@ -1645,12 +3975,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EE1DF64-B249-4492-AB46-334D22DB5578}">
-  <dimension ref="A1:AD3"/>
+  <dimension ref="A1:AD4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5"/>
@@ -1658,7 +3988,7 @@
     <col min="1" max="1" customWidth="true" width="24.5" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="16.1640625" collapsed="true"/>
     <col min="3" max="3" customWidth="true" width="52.5" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="38.6640625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="31.59375" collapsed="true"/>
     <col min="5" max="5" customWidth="true" width="22.6640625" collapsed="true"/>
     <col min="6" max="6" customWidth="true" width="20.1640625" collapsed="true"/>
     <col min="7" max="7" customWidth="true" width="24.5" collapsed="true"/>
@@ -1788,7 +4118,7 @@
         <v>130</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>158</v>
+        <v>403</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>97</v>
@@ -1864,234 +4194,24 @@
       </c>
     </row>
     <row r="3" spans="1:29">
+      <c r="D3" t="s">
+        <v>405</v>
+      </c>
       <c r="W3" s="6"/>
+    </row>
+    <row r="4">
+      <c r="D4" t="s">
+        <v>407</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21D1EA00-6B85-4E2C-9FB5-EA179A3143F2}">
-  <dimension ref="A1:H10"/>
-  <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5"/>
-  <cols>
-    <col min="1" max="1" customWidth="true" width="32.58203125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="31.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="17.33203125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="35.83203125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="42.4140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="28.1640625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="52.9140625" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>124</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79968134-293F-4959-B618-5F7E1CC36678}">
-  <dimension ref="A1:AC2"/>
+  <dimension ref="A1:AC4"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="AB2" sqref="AB2"/>
@@ -2102,7 +4222,7 @@
     <col min="1" max="1" customWidth="true" width="35.9140625" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="16.1640625" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="28.08203125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="42.58203125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="31.59375" collapsed="true"/>
     <col min="5" max="5" customWidth="true" width="29.33203125" collapsed="true"/>
     <col min="6" max="6" customWidth="true" width="23.83203125" collapsed="true"/>
     <col min="7" max="7" customWidth="true" width="29.33203125" collapsed="true"/>
@@ -2229,7 +4349,7 @@
         <v>132</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>96</v>
+        <v>403</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>97</v>
@@ -2299,6 +4419,16 @@
       </c>
       <c r="AA2" s="14" t="s">
         <v>129</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="D3" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="D4" t="s">
+        <v>407</v>
       </c>
     </row>
   </sheetData>
@@ -2306,9 +4436,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2BF8308-B45D-402E-AAF9-CB7AA6CDE09D}">
-  <dimension ref="A1:AS3"/>
+  <dimension ref="A1:AS4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
@@ -2317,9 +4447,9 @@
   <sheetFormatPr defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="20.1640625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="9.68359375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="27.27734375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="44.83203125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.6640625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="27.25" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="31.59375" collapsed="true"/>
     <col min="5" max="5" customWidth="true" width="24.08203125" collapsed="true"/>
     <col min="6" max="6" customWidth="true" width="20.6640625" collapsed="true"/>
     <col min="7" max="7" customWidth="true" width="22.9140625" collapsed="true"/>
@@ -2506,7 +4636,7 @@
         <v>169</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>158</v>
+        <v>403</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>97</v>
@@ -2630,7 +4760,9 @@
       </c>
     </row>
     <row r="3" spans="1:44">
-      <c r="D3" s="3"/>
+      <c r="D3" s="3" t="s">
+        <v>405</v>
+      </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -2668,12 +4800,17 @@
       <c r="AM3" s="2"/>
       <c r="AN3" s="2"/>
     </row>
+    <row r="4">
+      <c r="D4" t="s">
+        <v>407</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB4670CF-C1D6-4151-A4DE-06FECF44FB3D}">
   <dimension ref="A1:S7"/>
   <sheetViews>
@@ -2686,7 +4823,7 @@
     <col min="1" max="1" bestFit="true" customWidth="true" width="15.9140625" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="9.5" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="7.75" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="31.58203125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="31.59375" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="7.75" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="17.1640625" collapsed="true"/>
     <col min="7" max="7" bestFit="true" customWidth="true" width="20.4140625" collapsed="true"/>
@@ -2763,7 +4900,7 @@
         <v>95</v>
       </c>
       <c r="D2" t="s">
-        <v>158</v>
+        <v>403</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>97</v>
@@ -2806,6 +4943,16 @@
       </c>
       <c r="R2" s="6" t="s">
         <v>140</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="D3" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="D4" t="s">
+        <v>407</v>
       </c>
     </row>
     <row r="7" spans="1:18">
@@ -2817,7 +4964,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41BB444E-567D-443D-AA56-32CDE16C5EF4}">
   <dimension ref="A1:Z4"/>
   <sheetViews>
@@ -2830,7 +4977,7 @@
     <col min="1" max="1" bestFit="true" customWidth="true" width="15.9140625" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="9.6640625" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="18.08203125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="31.58203125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="31.59375" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="7.75" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="17.1640625" collapsed="true"/>
     <col min="7" max="7" bestFit="true" customWidth="true" width="23.58203125" collapsed="true"/>
@@ -2939,7 +5086,7 @@
         <v>147</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>96</v>
+        <v>403</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>97</v>
@@ -3008,7 +5155,9 @@
     <row r="3" spans="1:25">
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
+      <c r="D3" s="10" t="s">
+        <v>405</v>
+      </c>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
@@ -3028,7 +5177,9 @@
     <row r="4" spans="1:25">
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
+      <c r="D4" s="10" t="s">
+        <v>407</v>
+      </c>
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>

</xml_diff>